<commit_message>
v2 GPT-2 changes and pretrain and finetune results
</commit_message>
<xml_diff>
--- a/MyGPT2 Stats.xlsx
+++ b/MyGPT2 Stats.xlsx
@@ -8,25 +8,34 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vr/Code/LLMs/MyGPT2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{CB95715C-D871-FE4D-B2B4-4A19C4B82B82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{388D3883-4B2E-C547-B22F-1D5A8BB68762}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="800" windowWidth="41120" windowHeight="24660" activeTab="1" xr2:uid="{EE74674C-597E-C44B-9B9E-1DD01B1E9CF3}"/>
+    <workbookView xWindow="0" yWindow="800" windowWidth="41120" windowHeight="24680" activeTab="3" xr2:uid="{EE74674C-597E-C44B-9B9E-1DD01B1E9CF3}"/>
   </bookViews>
   <sheets>
     <sheet name="PreTrain" sheetId="1" r:id="rId1"/>
     <sheet name="FineTune" sheetId="2" r:id="rId2"/>
+    <sheet name="V2 Pretrain" sheetId="3" r:id="rId3"/>
+    <sheet name="V2 Pretrain-Bigger Model" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="_xlchart.v1.0" hidden="1">PreTrain!$E$1</definedName>
     <definedName name="_xlchart.v1.1" hidden="1">PreTrain!$E$2:$E$62</definedName>
+    <definedName name="_xlchart.v1.10" hidden="1">FineTune!$G$1</definedName>
+    <definedName name="_xlchart.v1.11" hidden="1">FineTune!$G$2:$G$12</definedName>
     <definedName name="_xlchart.v1.2" hidden="1">PreTrain!$E$1</definedName>
     <definedName name="_xlchart.v1.3" hidden="1">PreTrain!$E$2:$E$62</definedName>
     <definedName name="_xlchart.v1.4" hidden="1">PreTrain!$D$1</definedName>
     <definedName name="_xlchart.v1.5" hidden="1">PreTrain!$D$2:$D$62</definedName>
+    <definedName name="_xlchart.v1.6" hidden="1">FineTune!$C$2:$C$12</definedName>
+    <definedName name="_xlchart.v1.7" hidden="1">FineTune!$G$1</definedName>
+    <definedName name="_xlchart.v1.8" hidden="1">FineTune!$G$2:$G$12</definedName>
+    <definedName name="_xlchart.v1.9" hidden="1">FineTune!$C$2:$C$12</definedName>
+    <definedName name="_xlnm.Print_Titles" localSheetId="1">FineTune!$Q:$R,FineTune!$1:$2</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <pivotCaches>
-    <pivotCache cacheId="5" r:id="rId3"/>
+    <pivotCache cacheId="5" r:id="rId5"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -48,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="83">
   <si>
     <t>#</t>
   </si>
@@ -282,6 +291,21 @@
   </si>
   <si>
     <t>Size In KB</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> #</t>
+  </si>
+  <si>
+    <t>Book</t>
+  </si>
+  <si>
+    <t>Size KB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Time </t>
+  </si>
+  <si>
+    <t>elementary_illustrations_of_differential_and_integral_calculus</t>
   </si>
 </sst>
 </file>
@@ -312,7 +336,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -320,17 +344,37 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -346,6 +390,360 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>FineTune!$Q$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Time</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>FineTune!$P$2:$P$12</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>176</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>192</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>230</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>256</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>300</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>304</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>488</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>539</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>875</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>888</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1821</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>FineTune!$Q$2:$Q$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>9.1999999999999993</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>12.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>9.9</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>12.6</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>15.1</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>14.4</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>14.6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>14.8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>14.5</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>14.6</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>14</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-44C7-5948-8338-04B778AAE3F1}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1753292223"/>
+        <c:axId val="1753290431"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1753292223"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1753290431"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1753290431"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1753292223"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
 </file>
 
 <file path=xl/charts/chartEx1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -517,6 +915,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="366">
   <cs:axisTitle>
@@ -1529,6 +1967,522 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
   </cs:wall>
 </cs:chartStyle>
 </file>
@@ -1689,6 +2643,47 @@
         </xdr:sp>
       </mc:Fallback>
     </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>1028700</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>82550</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>63500</xdr:colOff>
+      <xdr:row>51</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="8" name="Chart 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E0459761-9D7A-E8D9-4AB4-8C7D436D4132}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -4855,10 +5850,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{657AAC80-72C3-3D4A-AF79-9F15624E8028}">
-  <dimension ref="A1:L12"/>
+  <dimension ref="A1:Q12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K7" sqref="K7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="P14" sqref="P14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4866,9 +5861,11 @@
     <col min="2" max="2" width="39.5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8.83203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8.1640625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="13" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="7.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4905,15 +5902,21 @@
       <c r="L1" s="1" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="P1" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
         <v>9</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="4">
         <f>VLOOKUP(B2,PreTrain!B2:D62,2,FALSE)</f>
         <v>875</v>
       </c>
@@ -4945,15 +5948,21 @@
       <c r="L2">
         <v>-1.341</v>
       </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="P2" s="4">
+        <v>176</v>
+      </c>
+      <c r="Q2">
+        <v>9.1999999999999993</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
         <v>10</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="4">
         <f>VLOOKUP(B3,PreTrain!B3:D63,2,FALSE)</f>
         <v>176</v>
       </c>
@@ -4985,15 +5994,21 @@
       <c r="L3">
         <v>0.1444</v>
       </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="P3" s="4">
+        <v>192</v>
+      </c>
+      <c r="Q3">
+        <v>12.5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
         <v>11</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="4">
         <f>VLOOKUP(B4,PreTrain!B4:D64,2,FALSE)</f>
         <v>888</v>
       </c>
@@ -5025,15 +6040,21 @@
       <c r="L4">
         <v>-1.2212000000000001</v>
       </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="P4" s="4">
+        <v>230</v>
+      </c>
+      <c r="Q4">
+        <v>9.9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
         <v>14</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="4">
         <f>VLOOKUP(B5,PreTrain!B5:D65,2,FALSE)</f>
         <v>304</v>
       </c>
@@ -5065,15 +6086,21 @@
       <c r="L5">
         <v>-2.3298999999999999</v>
       </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="P5" s="4">
+        <v>256</v>
+      </c>
+      <c r="Q5">
+        <v>12.6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" t="s">
         <v>17</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="4">
         <f>VLOOKUP(B6,PreTrain!B6:D66,2,FALSE)</f>
         <v>256</v>
       </c>
@@ -5105,15 +6132,21 @@
       <c r="L6">
         <v>-0.53520000000000001</v>
       </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="P6" s="4">
+        <v>300</v>
+      </c>
+      <c r="Q6">
+        <v>15.1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" t="s">
         <v>28</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="4">
         <f>VLOOKUP(B7,PreTrain!B7:D67,2,FALSE)</f>
         <v>1821</v>
       </c>
@@ -5145,15 +6178,21 @@
       <c r="L7">
         <v>-2.2913999999999999</v>
       </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="P7" s="4">
+        <v>304</v>
+      </c>
+      <c r="Q7">
+        <v>14.4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8" t="s">
         <v>30</v>
       </c>
-      <c r="C8">
+      <c r="C8" s="4">
         <f>VLOOKUP(B8,PreTrain!B8:D68,2,FALSE)</f>
         <v>300</v>
       </c>
@@ -5185,15 +6224,21 @@
       <c r="L8">
         <v>-1.9419</v>
       </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="P8" s="4">
+        <v>488</v>
+      </c>
+      <c r="Q8">
+        <v>14.6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9" t="s">
         <v>37</v>
       </c>
-      <c r="C9">
+      <c r="C9" s="4">
         <f>VLOOKUP(B9,PreTrain!B9:D69,2,FALSE)</f>
         <v>539</v>
       </c>
@@ -5225,15 +6270,21 @@
       <c r="L9">
         <v>-2.8029999999999999</v>
       </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="P9" s="4">
+        <v>539</v>
+      </c>
+      <c r="Q9">
+        <v>14.8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="B10" t="s">
         <v>39</v>
       </c>
-      <c r="C10">
+      <c r="C10" s="4">
         <f>VLOOKUP(B10,PreTrain!B10:D70,2,FALSE)</f>
         <v>488</v>
       </c>
@@ -5265,15 +6316,21 @@
       <c r="L10">
         <v>-2.3409</v>
       </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="P10" s="4">
+        <v>875</v>
+      </c>
+      <c r="Q10">
+        <v>14.5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>10</v>
       </c>
       <c r="B11" t="s">
         <v>40</v>
       </c>
-      <c r="C11">
+      <c r="C11" s="4">
         <f>VLOOKUP(B11,PreTrain!B11:D71,2,FALSE)</f>
         <v>230</v>
       </c>
@@ -5305,15 +6362,21 @@
       <c r="L11">
         <v>0.77949999999999997</v>
       </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="P11" s="4">
+        <v>888</v>
+      </c>
+      <c r="Q11">
+        <v>14.6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>11</v>
       </c>
       <c r="B12" t="s">
         <v>41</v>
       </c>
-      <c r="C12">
+      <c r="C12" s="4">
         <f>VLOOKUP(B12,PreTrain!B12:D72,2,FALSE)</f>
         <v>192</v>
       </c>
@@ -5344,6 +6407,1629 @@
       </c>
       <c r="L12">
         <v>-1.96</v>
+      </c>
+      <c r="P12" s="4">
+        <v>1821</v>
+      </c>
+      <c r="Q12">
+        <v>14</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="P2:Q12">
+    <sortCondition ref="P2:P12"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B071073B-22D5-954D-8BD2-42AD2F281A7F}">
+  <dimension ref="A1:J18"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="3.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="56.1640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>15</v>
+      </c>
+      <c r="B2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C2">
+        <v>230</v>
+      </c>
+      <c r="D2">
+        <v>235706</v>
+      </c>
+      <c r="E2">
+        <v>56</v>
+      </c>
+      <c r="F2">
+        <v>7.8</v>
+      </c>
+      <c r="G2">
+        <v>8.4</v>
+      </c>
+      <c r="H2">
+        <v>3.1442999999999999</v>
+      </c>
+      <c r="I2">
+        <v>23.2</v>
+      </c>
+      <c r="J2">
+        <v>2.9939</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3">
+        <v>176</v>
+      </c>
+      <c r="D3">
+        <v>179877</v>
+      </c>
+      <c r="E3">
+        <v>57</v>
+      </c>
+      <c r="F3">
+        <v>6.4</v>
+      </c>
+      <c r="G3">
+        <v>6.7</v>
+      </c>
+      <c r="H3">
+        <v>3.4885999999999999</v>
+      </c>
+      <c r="I3">
+        <v>32.700000000000003</v>
+      </c>
+      <c r="J3">
+        <v>3.2818999999999998</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>7</v>
+      </c>
+      <c r="B4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C4">
+        <v>320</v>
+      </c>
+      <c r="D4">
+        <v>326972</v>
+      </c>
+      <c r="E4">
+        <v>47</v>
+      </c>
+      <c r="F4">
+        <v>8.6</v>
+      </c>
+      <c r="G4">
+        <v>11</v>
+      </c>
+      <c r="H4">
+        <v>4.5491000000000001</v>
+      </c>
+      <c r="I4">
+        <v>94.5</v>
+      </c>
+      <c r="J4">
+        <v>3.3159000000000001</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>1</v>
+      </c>
+      <c r="B5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5">
+        <v>875</v>
+      </c>
+      <c r="D5">
+        <v>895837</v>
+      </c>
+      <c r="E5">
+        <v>40</v>
+      </c>
+      <c r="F5">
+        <v>16.899999999999999</v>
+      </c>
+      <c r="G5">
+        <v>25.3</v>
+      </c>
+      <c r="H5">
+        <v>4.9401999999999999</v>
+      </c>
+      <c r="I5">
+        <v>139.80000000000001</v>
+      </c>
+      <c r="J5">
+        <v>3.2305999999999999</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>17</v>
+      </c>
+      <c r="B6" t="s">
+        <v>47</v>
+      </c>
+      <c r="C6">
+        <v>123</v>
+      </c>
+      <c r="D6">
+        <v>125756</v>
+      </c>
+      <c r="E6">
+        <v>62</v>
+      </c>
+      <c r="F6">
+        <v>3.4</v>
+      </c>
+      <c r="G6">
+        <v>3.2</v>
+      </c>
+      <c r="H6">
+        <v>5.2096</v>
+      </c>
+      <c r="I6">
+        <v>183</v>
+      </c>
+      <c r="J6">
+        <v>3.5607000000000002</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>11</v>
+      </c>
+      <c r="B7" t="s">
+        <v>29</v>
+      </c>
+      <c r="C7">
+        <v>1129</v>
+      </c>
+      <c r="D7">
+        <v>1112062</v>
+      </c>
+      <c r="E7">
+        <v>32</v>
+      </c>
+      <c r="F7">
+        <v>16.8</v>
+      </c>
+      <c r="G7">
+        <v>31.5</v>
+      </c>
+      <c r="H7">
+        <v>5.2896000000000001</v>
+      </c>
+      <c r="I7">
+        <v>198.3</v>
+      </c>
+      <c r="J7">
+        <v>3.9117000000000002</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>5</v>
+      </c>
+      <c r="B8" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8">
+        <v>256</v>
+      </c>
+      <c r="D8">
+        <v>261740</v>
+      </c>
+      <c r="E8">
+        <v>56</v>
+      </c>
+      <c r="F8">
+        <v>7</v>
+      </c>
+      <c r="G8">
+        <v>7.5</v>
+      </c>
+      <c r="H8">
+        <v>5.3315999999999999</v>
+      </c>
+      <c r="I8">
+        <v>206.8</v>
+      </c>
+      <c r="J8">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>3</v>
+      </c>
+      <c r="B9" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9">
+        <v>888</v>
+      </c>
+      <c r="D9">
+        <v>908238</v>
+      </c>
+      <c r="E9">
+        <v>36</v>
+      </c>
+      <c r="F9">
+        <v>13</v>
+      </c>
+      <c r="G9">
+        <v>21.6</v>
+      </c>
+      <c r="H9">
+        <v>5.8648999999999996</v>
+      </c>
+      <c r="I9">
+        <v>352.4</v>
+      </c>
+      <c r="J9">
+        <v>4.5705</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>14</v>
+      </c>
+      <c r="B10" t="s">
+        <v>39</v>
+      </c>
+      <c r="C10">
+        <v>488</v>
+      </c>
+      <c r="D10">
+        <v>500054</v>
+      </c>
+      <c r="E10">
+        <v>46</v>
+      </c>
+      <c r="F10">
+        <v>9.1999999999999993</v>
+      </c>
+      <c r="G10">
+        <v>12</v>
+      </c>
+      <c r="H10">
+        <v>6.1505000000000001</v>
+      </c>
+      <c r="I10">
+        <v>469</v>
+      </c>
+      <c r="J10">
+        <v>3.6328999999999998</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>28</v>
+      </c>
+      <c r="C11">
+        <v>1821</v>
+      </c>
+      <c r="D11">
+        <v>1854300</v>
+      </c>
+      <c r="E11">
+        <v>37</v>
+      </c>
+      <c r="F11">
+        <v>22.9</v>
+      </c>
+      <c r="G11">
+        <v>37.200000000000003</v>
+      </c>
+      <c r="H11">
+        <v>6.1936999999999998</v>
+      </c>
+      <c r="I11">
+        <v>489.7</v>
+      </c>
+      <c r="J11">
+        <v>3.5203000000000002</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>16</v>
+      </c>
+      <c r="B12" t="s">
+        <v>41</v>
+      </c>
+      <c r="C12">
+        <v>192</v>
+      </c>
+      <c r="D12">
+        <v>196822</v>
+      </c>
+      <c r="E12">
+        <v>65</v>
+      </c>
+      <c r="F12">
+        <v>5</v>
+      </c>
+      <c r="G12">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="H12">
+        <v>6.2614000000000001</v>
+      </c>
+      <c r="I12">
+        <v>524</v>
+      </c>
+      <c r="J12">
+        <v>4.0734000000000004</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>30</v>
+      </c>
+      <c r="C13">
+        <v>300</v>
+      </c>
+      <c r="D13">
+        <v>306401</v>
+      </c>
+      <c r="E13">
+        <v>50</v>
+      </c>
+      <c r="F13">
+        <v>6.3</v>
+      </c>
+      <c r="G13">
+        <v>7.6</v>
+      </c>
+      <c r="H13">
+        <v>6.3728999999999996</v>
+      </c>
+      <c r="I13">
+        <v>585.79999999999995</v>
+      </c>
+      <c r="J13">
+        <v>3.637</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>9</v>
+      </c>
+      <c r="B14" t="s">
+        <v>26</v>
+      </c>
+      <c r="C14">
+        <v>816</v>
+      </c>
+      <c r="D14">
+        <v>835629</v>
+      </c>
+      <c r="E14">
+        <v>37</v>
+      </c>
+      <c r="F14">
+        <v>12.5</v>
+      </c>
+      <c r="G14">
+        <v>20.3</v>
+      </c>
+      <c r="H14">
+        <v>6.6512000000000002</v>
+      </c>
+      <c r="I14">
+        <v>773.7</v>
+      </c>
+      <c r="J14">
+        <v>4.5027999999999997</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>8</v>
+      </c>
+      <c r="B15" t="s">
+        <v>25</v>
+      </c>
+      <c r="C15">
+        <v>236</v>
+      </c>
+      <c r="D15">
+        <v>241092</v>
+      </c>
+      <c r="E15">
+        <v>66</v>
+      </c>
+      <c r="F15">
+        <v>5.9</v>
+      </c>
+      <c r="G15">
+        <v>5.3</v>
+      </c>
+      <c r="H15">
+        <v>6.9974999999999996</v>
+      </c>
+      <c r="I15">
+        <v>1093.9000000000001</v>
+      </c>
+      <c r="J15">
+        <v>4.7393999999999998</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>6</v>
+      </c>
+      <c r="B16" t="s">
+        <v>18</v>
+      </c>
+      <c r="C16">
+        <v>240</v>
+      </c>
+      <c r="D16">
+        <v>245888</v>
+      </c>
+      <c r="E16">
+        <v>64</v>
+      </c>
+      <c r="F16">
+        <v>6.4</v>
+      </c>
+      <c r="G16">
+        <v>6</v>
+      </c>
+      <c r="H16">
+        <v>7.0538999999999996</v>
+      </c>
+      <c r="I16">
+        <v>1157.4000000000001</v>
+      </c>
+      <c r="J16">
+        <v>4.4927000000000001</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>13</v>
+      </c>
+      <c r="B17" t="s">
+        <v>37</v>
+      </c>
+      <c r="C17">
+        <v>539</v>
+      </c>
+      <c r="D17">
+        <v>552041</v>
+      </c>
+      <c r="E17">
+        <v>36</v>
+      </c>
+      <c r="F17">
+        <v>8.5</v>
+      </c>
+      <c r="G17">
+        <v>14.1</v>
+      </c>
+      <c r="H17">
+        <v>7.1444999999999999</v>
+      </c>
+      <c r="I17">
+        <v>1267.2</v>
+      </c>
+      <c r="J17">
+        <v>4.1821000000000002</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>4</v>
+      </c>
+      <c r="B18" t="s">
+        <v>14</v>
+      </c>
+      <c r="C18">
+        <v>304</v>
+      </c>
+      <c r="D18">
+        <v>310852</v>
+      </c>
+      <c r="E18">
+        <v>23</v>
+      </c>
+      <c r="F18">
+        <v>2.7</v>
+      </c>
+      <c r="G18">
+        <v>7</v>
+      </c>
+      <c r="H18">
+        <v>7.4965000000000002</v>
+      </c>
+      <c r="I18">
+        <v>1801.8</v>
+      </c>
+      <c r="J18">
+        <v>6.0880999999999998</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:J18">
+    <sortCondition ref="I2:I18"/>
+    <sortCondition ref="H2:H18"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FBB6F03C-FBB2-9641-B5FD-7C3591998950}">
+  <dimension ref="A1:G43"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="K40" sqref="K40"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="6.6640625" customWidth="1"/>
+    <col min="2" max="2" width="52.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12" customWidth="1"/>
+    <col min="4" max="4" width="13.5" customWidth="1"/>
+    <col min="5" max="5" width="15" customWidth="1"/>
+    <col min="6" max="6" width="11.83203125" customWidth="1"/>
+    <col min="7" max="7" width="9.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2" s="6">
+        <v>1</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" s="6">
+        <v>18</v>
+      </c>
+      <c r="D2" s="6">
+        <v>3.4000000000000002E-2</v>
+      </c>
+      <c r="E2" s="6">
+        <v>1</v>
+      </c>
+      <c r="F2" s="6">
+        <v>100</v>
+      </c>
+      <c r="G2" s="6">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3" s="6">
+        <v>2</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="C3" s="6">
+        <v>230</v>
+      </c>
+      <c r="D3" s="6">
+        <v>3.1442999999999999</v>
+      </c>
+      <c r="E3" s="6">
+        <v>23.2</v>
+      </c>
+      <c r="F3" s="6">
+        <v>71</v>
+      </c>
+      <c r="G3" s="6">
+        <v>9.1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4" s="6">
+        <v>3</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="6">
+        <v>176</v>
+      </c>
+      <c r="D4" s="6">
+        <v>3.488</v>
+      </c>
+      <c r="E4" s="6">
+        <v>32.700000000000003</v>
+      </c>
+      <c r="F4" s="6">
+        <v>70</v>
+      </c>
+      <c r="G4" s="6">
+        <v>7.4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5" s="6">
+        <v>4</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="C5" s="6">
+        <v>335</v>
+      </c>
+      <c r="D5" s="6">
+        <v>4.5144000000000002</v>
+      </c>
+      <c r="E5" s="6">
+        <v>91.3</v>
+      </c>
+      <c r="F5" s="6">
+        <v>77</v>
+      </c>
+      <c r="G5" s="6">
+        <v>13.6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6" s="6">
+        <v>5</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C6" s="6">
+        <v>71</v>
+      </c>
+      <c r="D6" s="6">
+        <v>4.5231000000000003</v>
+      </c>
+      <c r="E6" s="6">
+        <v>92.1</v>
+      </c>
+      <c r="F6" s="6">
+        <v>72</v>
+      </c>
+      <c r="G6" s="6">
+        <v>1.8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7" s="6">
+        <v>6</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C7" s="6">
+        <v>320</v>
+      </c>
+      <c r="D7" s="6">
+        <v>4.5500999999999996</v>
+      </c>
+      <c r="E7" s="6">
+        <v>94.6</v>
+      </c>
+      <c r="F7" s="6">
+        <v>62</v>
+      </c>
+      <c r="G7" s="6">
+        <v>10.3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A8" s="6">
+        <v>7</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" s="6">
+        <v>875</v>
+      </c>
+      <c r="D8" s="6">
+        <v>4.9401999999999999</v>
+      </c>
+      <c r="E8" s="6">
+        <v>139.80000000000001</v>
+      </c>
+      <c r="F8" s="6">
+        <v>55</v>
+      </c>
+      <c r="G8" s="6">
+        <v>21.7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A9" s="6">
+        <v>8</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="C9" s="6">
+        <v>123</v>
+      </c>
+      <c r="D9" s="6">
+        <v>5.2046000000000001</v>
+      </c>
+      <c r="E9" s="6">
+        <v>182.1</v>
+      </c>
+      <c r="F9" s="6">
+        <v>81</v>
+      </c>
+      <c r="G9" s="6">
+        <v>3.9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A10" s="6">
+        <v>9</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C10" s="6">
+        <v>342</v>
+      </c>
+      <c r="D10" s="6">
+        <v>5.2679999999999998</v>
+      </c>
+      <c r="E10" s="6">
+        <v>194</v>
+      </c>
+      <c r="F10" s="6">
+        <v>64</v>
+      </c>
+      <c r="G10" s="6">
+        <v>8.1999999999999993</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A11" s="6">
+        <v>10</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C11" s="6">
+        <v>1129</v>
+      </c>
+      <c r="D11" s="6">
+        <v>5.2834000000000003</v>
+      </c>
+      <c r="E11" s="6">
+        <v>197</v>
+      </c>
+      <c r="F11" s="6">
+        <v>50</v>
+      </c>
+      <c r="G11" s="6">
+        <v>24.5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A12" s="6">
+        <v>11</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="C12" s="6">
+        <v>134</v>
+      </c>
+      <c r="D12" s="6">
+        <v>5.3068</v>
+      </c>
+      <c r="E12" s="6">
+        <v>201.7</v>
+      </c>
+      <c r="F12" s="6">
+        <v>69</v>
+      </c>
+      <c r="G12" s="6">
+        <v>3.3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A13" s="6">
+        <v>12</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C13" s="6">
+        <v>256</v>
+      </c>
+      <c r="D13" s="6">
+        <v>5.3224</v>
+      </c>
+      <c r="E13" s="6">
+        <v>204.9</v>
+      </c>
+      <c r="F13" s="6">
+        <v>80</v>
+      </c>
+      <c r="G13" s="6">
+        <v>9.6</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A14" s="6">
+        <v>13</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="C14" s="6">
+        <v>302</v>
+      </c>
+      <c r="D14" s="6">
+        <v>5.4169</v>
+      </c>
+      <c r="E14" s="6">
+        <v>225.2</v>
+      </c>
+      <c r="F14" s="6">
+        <v>67</v>
+      </c>
+      <c r="G14" s="6">
+        <v>7.8</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A15" s="6">
+        <v>14</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="C15" s="6">
+        <v>161</v>
+      </c>
+      <c r="D15" s="6">
+        <v>5.4652000000000003</v>
+      </c>
+      <c r="E15" s="6">
+        <v>236.3</v>
+      </c>
+      <c r="F15" s="6">
+        <v>82</v>
+      </c>
+      <c r="G15" s="6">
+        <v>4.9000000000000004</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A16" s="6">
+        <v>15</v>
+      </c>
+      <c r="B16" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C16" s="6">
+        <v>888</v>
+      </c>
+      <c r="D16" s="6">
+        <v>5.8551000000000002</v>
+      </c>
+      <c r="E16" s="6">
+        <v>349</v>
+      </c>
+      <c r="F16" s="6">
+        <v>55</v>
+      </c>
+      <c r="G16" s="6">
+        <v>18.5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A17" s="6">
+        <v>16</v>
+      </c>
+      <c r="B17" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="C17" s="6">
+        <v>73</v>
+      </c>
+      <c r="D17" s="6">
+        <v>5.8795000000000002</v>
+      </c>
+      <c r="E17" s="6">
+        <v>357.6</v>
+      </c>
+      <c r="F17" s="6">
+        <v>65</v>
+      </c>
+      <c r="G17" s="6">
+        <v>1.6</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A18" s="6">
+        <v>17</v>
+      </c>
+      <c r="B18" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C18" s="6">
+        <v>472</v>
+      </c>
+      <c r="D18" s="6">
+        <v>6.0125000000000002</v>
+      </c>
+      <c r="E18" s="6">
+        <v>408.5</v>
+      </c>
+      <c r="F18" s="6">
+        <v>72</v>
+      </c>
+      <c r="G18" s="6">
+        <v>10.9</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A19" s="6">
+        <v>18</v>
+      </c>
+      <c r="B19" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C19" s="6">
+        <v>770</v>
+      </c>
+      <c r="D19" s="6">
+        <v>6.0641999999999996</v>
+      </c>
+      <c r="E19" s="6">
+        <v>430.2</v>
+      </c>
+      <c r="F19" s="6">
+        <v>54</v>
+      </c>
+      <c r="G19" s="6">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A20" s="6">
+        <v>19</v>
+      </c>
+      <c r="B20" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="C20" s="6">
+        <v>209</v>
+      </c>
+      <c r="D20" s="6">
+        <v>6.0673000000000004</v>
+      </c>
+      <c r="E20" s="6">
+        <v>431.5</v>
+      </c>
+      <c r="F20" s="6">
+        <v>90</v>
+      </c>
+      <c r="G20" s="6">
+        <v>7.4</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A21" s="6">
+        <v>20</v>
+      </c>
+      <c r="B21" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="C21" s="6">
+        <v>124</v>
+      </c>
+      <c r="D21" s="6">
+        <v>6.1220999999999997</v>
+      </c>
+      <c r="E21" s="6">
+        <v>455.8</v>
+      </c>
+      <c r="F21" s="6">
+        <v>88</v>
+      </c>
+      <c r="G21" s="6">
+        <v>4.2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A22" s="6">
+        <v>21</v>
+      </c>
+      <c r="B22" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="C22" s="6">
+        <v>488</v>
+      </c>
+      <c r="D22" s="6">
+        <v>6.1505000000000001</v>
+      </c>
+      <c r="E22" s="6">
+        <v>469</v>
+      </c>
+      <c r="F22" s="6">
+        <v>61</v>
+      </c>
+      <c r="G22" s="6">
+        <v>11.3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A23" s="6">
+        <v>22</v>
+      </c>
+      <c r="B23" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="C23" s="6">
+        <v>209</v>
+      </c>
+      <c r="D23" s="6">
+        <v>6.1542000000000003</v>
+      </c>
+      <c r="E23" s="6">
+        <v>470.7</v>
+      </c>
+      <c r="F23" s="6">
+        <v>78</v>
+      </c>
+      <c r="G23" s="6">
+        <v>7.3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A24" s="6">
+        <v>23</v>
+      </c>
+      <c r="B24" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C24" s="6">
+        <v>1821</v>
+      </c>
+      <c r="D24" s="6">
+        <v>6.1936999999999998</v>
+      </c>
+      <c r="E24" s="6">
+        <v>489.7</v>
+      </c>
+      <c r="F24" s="6">
+        <v>52</v>
+      </c>
+      <c r="G24" s="6">
+        <v>29.6</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A25" s="6">
+        <v>24</v>
+      </c>
+      <c r="B25" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="C25" s="6">
+        <v>192</v>
+      </c>
+      <c r="D25" s="6">
+        <v>6.2614000000000001</v>
+      </c>
+      <c r="E25" s="6">
+        <v>523.9</v>
+      </c>
+      <c r="F25" s="6">
+        <v>80</v>
+      </c>
+      <c r="G25" s="6">
+        <v>5.6</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A26" s="6">
+        <v>25</v>
+      </c>
+      <c r="B26" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C26" s="6">
+        <v>192</v>
+      </c>
+      <c r="D26" s="6">
+        <v>6.2713000000000001</v>
+      </c>
+      <c r="E26" s="6">
+        <v>529.20000000000005</v>
+      </c>
+      <c r="F26" s="6">
+        <v>67</v>
+      </c>
+      <c r="G26" s="6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A27" s="6">
+        <v>26</v>
+      </c>
+      <c r="B27" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C27" s="6">
+        <v>171</v>
+      </c>
+      <c r="D27" s="6">
+        <v>6.2971000000000004</v>
+      </c>
+      <c r="E27" s="6">
+        <v>543</v>
+      </c>
+      <c r="F27" s="6">
+        <v>81</v>
+      </c>
+      <c r="G27" s="6">
+        <v>4.8</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A28" s="6">
+        <v>27</v>
+      </c>
+      <c r="B28" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="C28" s="6">
+        <v>101</v>
+      </c>
+      <c r="D28" s="6">
+        <v>6.3178000000000001</v>
+      </c>
+      <c r="E28" s="6">
+        <v>554.4</v>
+      </c>
+      <c r="F28" s="6">
+        <v>73</v>
+      </c>
+      <c r="G28" s="6">
+        <v>1.8</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A29" s="6">
+        <v>28</v>
+      </c>
+      <c r="B29" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="C29" s="6">
+        <v>54</v>
+      </c>
+      <c r="D29" s="6">
+        <v>6.3273000000000001</v>
+      </c>
+      <c r="E29" s="6">
+        <v>559.6</v>
+      </c>
+      <c r="F29" s="6">
+        <v>56</v>
+      </c>
+      <c r="G29" s="6">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A30" s="6">
+        <v>29</v>
+      </c>
+      <c r="B30" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="C30" s="6">
+        <v>300</v>
+      </c>
+      <c r="D30" s="6">
+        <v>6.3566000000000003</v>
+      </c>
+      <c r="E30" s="6">
+        <v>576.29999999999995</v>
+      </c>
+      <c r="F30" s="6">
+        <v>81</v>
+      </c>
+      <c r="G30" s="6">
+        <v>9.4</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A31" s="6">
+        <v>30</v>
+      </c>
+      <c r="B31" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="C31" s="6">
+        <v>954</v>
+      </c>
+      <c r="D31" s="6">
+        <v>6.3631000000000002</v>
+      </c>
+      <c r="E31" s="6">
+        <v>580</v>
+      </c>
+      <c r="F31" s="6">
+        <v>64</v>
+      </c>
+      <c r="G31" s="6">
+        <v>19.3</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A32" s="6">
+        <v>31</v>
+      </c>
+      <c r="B32" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="C32" s="6">
+        <v>218</v>
+      </c>
+      <c r="D32" s="6">
+        <v>6.3746999999999998</v>
+      </c>
+      <c r="E32" s="6">
+        <v>586.79999999999995</v>
+      </c>
+      <c r="F32" s="6">
+        <v>78</v>
+      </c>
+      <c r="G32" s="6">
+        <v>6.4</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A33" s="6">
+        <v>32</v>
+      </c>
+      <c r="B33" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="C33" s="6">
+        <v>348</v>
+      </c>
+      <c r="D33" s="6">
+        <v>6.6113</v>
+      </c>
+      <c r="E33" s="6">
+        <v>743.4</v>
+      </c>
+      <c r="F33" s="6">
+        <v>62</v>
+      </c>
+      <c r="G33" s="6">
+        <v>9.4</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A34" s="6">
+        <v>33</v>
+      </c>
+      <c r="B34" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="C34" s="6">
+        <v>359</v>
+      </c>
+      <c r="D34" s="6">
+        <v>6.6264000000000003</v>
+      </c>
+      <c r="E34" s="6">
+        <v>754.8</v>
+      </c>
+      <c r="F34" s="6">
+        <v>68</v>
+      </c>
+      <c r="G34" s="6">
+        <v>7.9</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A35" s="6">
+        <v>34</v>
+      </c>
+      <c r="B35" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="C35" s="6">
+        <v>816</v>
+      </c>
+      <c r="D35" s="6">
+        <v>6.6448999999999998</v>
+      </c>
+      <c r="E35" s="6">
+        <v>768.9</v>
+      </c>
+      <c r="F35" s="6">
+        <v>54</v>
+      </c>
+      <c r="G35" s="6">
+        <v>16.600000000000001</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A36" s="6">
+        <v>35</v>
+      </c>
+      <c r="B36" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="C36" s="6">
+        <v>400</v>
+      </c>
+      <c r="D36" s="6">
+        <v>6.7309000000000001</v>
+      </c>
+      <c r="E36" s="6">
+        <v>837.9</v>
+      </c>
+      <c r="F36" s="6">
+        <v>59</v>
+      </c>
+      <c r="G36" s="6">
+        <v>8.9</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A37" s="6">
+        <v>36</v>
+      </c>
+      <c r="B37" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="C37" s="6">
+        <v>88</v>
+      </c>
+      <c r="D37" s="6">
+        <v>6.7523999999999997</v>
+      </c>
+      <c r="E37" s="6">
+        <v>856.1</v>
+      </c>
+      <c r="F37" s="6">
+        <v>53</v>
+      </c>
+      <c r="G37" s="6">
+        <v>1.9</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A38" s="6">
+        <v>37</v>
+      </c>
+      <c r="B38" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="C38" s="6">
+        <v>180</v>
+      </c>
+      <c r="D38" s="6">
+        <v>6.9276</v>
+      </c>
+      <c r="E38" s="6">
+        <v>1020.1</v>
+      </c>
+      <c r="F38" s="6">
+        <v>73</v>
+      </c>
+      <c r="G38" s="6">
+        <v>4.3</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A39" s="6">
+        <v>38</v>
+      </c>
+      <c r="B39" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="C39" s="6">
+        <v>236</v>
+      </c>
+      <c r="D39" s="6">
+        <v>6.9893000000000001</v>
+      </c>
+      <c r="E39" s="6">
+        <v>1084.9000000000001</v>
+      </c>
+      <c r="F39" s="6">
+        <v>82</v>
+      </c>
+      <c r="G39" s="6">
+        <v>7.2</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A40" s="6">
+        <v>39</v>
+      </c>
+      <c r="B40" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C40" s="6">
+        <v>166</v>
+      </c>
+      <c r="D40" s="6">
+        <v>7.0072000000000001</v>
+      </c>
+      <c r="E40" s="6">
+        <v>1104.5</v>
+      </c>
+      <c r="F40" s="6">
+        <v>64</v>
+      </c>
+      <c r="G40" s="6">
+        <v>3.8</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A41" s="6">
+        <v>40</v>
+      </c>
+      <c r="B41" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="C41" s="6">
+        <v>240</v>
+      </c>
+      <c r="D41" s="6">
+        <v>7.0538999999999996</v>
+      </c>
+      <c r="E41" s="6">
+        <v>1157.4000000000001</v>
+      </c>
+      <c r="F41" s="6">
+        <v>79</v>
+      </c>
+      <c r="G41" s="6">
+        <v>7.9</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A42" s="6">
+        <v>41</v>
+      </c>
+      <c r="B42" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="C42" s="6">
+        <v>539</v>
+      </c>
+      <c r="D42" s="6">
+        <v>7.1444999999999999</v>
+      </c>
+      <c r="E42" s="6">
+        <v>1267.2</v>
+      </c>
+      <c r="F42" s="6">
+        <v>51</v>
+      </c>
+      <c r="G42" s="6">
+        <v>11.2</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A43" s="6">
+        <v>42</v>
+      </c>
+      <c r="B43" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C43" s="6">
+        <v>304</v>
+      </c>
+      <c r="D43" s="6">
+        <v>7.4516999999999998</v>
+      </c>
+      <c r="E43" s="6">
+        <v>1722.7</v>
+      </c>
+      <c r="F43" s="6">
+        <v>98</v>
+      </c>
+      <c r="G43" s="6">
+        <v>10.199999999999999</v>
       </c>
     </row>
   </sheetData>

</xml_diff>